<commit_message>
this is second commit of new change
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">january </t>
+  </si>
+  <si>
+    <t>february</t>
+  </si>
+  <si>
+    <t>march</t>
+  </si>
+  <si>
+    <t>april</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>june</t>
+  </si>
+  <si>
+    <t>july</t>
+  </si>
+  <si>
+    <t>august</t>
+  </si>
+  <si>
+    <t>september</t>
+  </si>
+  <si>
+    <t>october</t>
+  </si>
+  <si>
+    <t>november</t>
+  </si>
+  <si>
+    <t>december</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +114,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +411,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>